<commit_message>
Edited the test template
Made it for the three filters:
Wavelet
FIRR
IIR
</commit_message>
<xml_diff>
--- a/Testing/testing results.xlsx
+++ b/Testing/testing results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\The 9 sins\final\The_9Sines\Testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB67D5E-4AE1-4A1C-9255-4A931C9E3430}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827FA72F-E2E5-45C5-8C1D-E245FBE1CDAC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648" xr2:uid="{3948DF21-CB8A-4613-ADA3-C1805D9B1523}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="10">
   <si>
     <t>MSE</t>
   </si>
@@ -47,12 +47,21 @@
   <si>
     <t>MSE avg</t>
   </si>
+  <si>
+    <t>Wavelet</t>
+  </si>
+  <si>
+    <t>FIR</t>
+  </si>
+  <si>
+    <t>IIR</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +72,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -88,7 +105,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -97,6 +114,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -157,7 +180,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>MSE-PSNR</a:t>
+              <a:t>Wavelet</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1340,7 +1363,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Avg</a:t>
+              <a:t>FIR</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1392,11 +1415,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$10</c:f>
+              <c:f>Sheet1!$C$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> PSNR avg</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1405,21 +1428,21 @@
             <a:gradFill rotWithShape="1">
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:schemeClr val="accent6">
+                  <a:schemeClr val="accent1">
                     <a:satMod val="103000"/>
                     <a:lumMod val="102000"/>
                     <a:tint val="94000"/>
                   </a:schemeClr>
                 </a:gs>
                 <a:gs pos="50000">
-                  <a:schemeClr val="accent6">
+                  <a:schemeClr val="accent1">
                     <a:satMod val="110000"/>
                     <a:lumMod val="100000"/>
                     <a:shade val="100000"/>
                   </a:schemeClr>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:schemeClr val="accent6">
+                  <a:schemeClr val="accent1">
                     <a:lumMod val="99000"/>
                     <a:satMod val="120000"/>
                     <a:shade val="78000"/>
@@ -1440,44 +1463,128 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$K$11:$K$13</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Normal</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>High</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$41:$B$46</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$11:$L$13</c:f>
+              <c:f>Sheet1!$C$41:$C$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>265.2</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>302.60000000000002</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>437.6</c:v>
+                  <c:v>627</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-91CE-445A-B54C-6ED0FCA6379C}"/>
+              <c16:uniqueId val="{00000000-55D3-4089-BA37-53FBB933CF3E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1486,11 +1593,545 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$10</c:f>
+              <c:f>Sheet1!$D$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MSE avg</c:v>
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$41:$B$46</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$41:$D$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>735</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-55D3-4089-BA37-53FBB933CF3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$41:$B$46</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$41:$E$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>390</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-55D3-4089-BA37-53FBB933CF3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$41:$B$46</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$41:$F$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-55D3-4089-BA37-53FBB933CF3E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1534,50 +2175,135 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$K$11:$K$13</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Normal</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>High</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$41:$B$46</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$11:$M$13</c:f>
+              <c:f>Sheet1!$G$41:$G$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>567.20000000000005</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>529</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>383.4</c:v>
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-91CE-445A-B54C-6ED0FCA6379C}"/>
+              <c16:uniqueId val="{00000004-55D3-4089-BA37-53FBB933CF3E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1585,11 +2311,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="576392120"/>
-        <c:axId val="576396712"/>
+        <c:axId val="564851664"/>
+        <c:axId val="564858880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="576392120"/>
+        <c:axId val="564851664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1631,7 +2357,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="576396712"/>
+        <c:crossAx val="564858880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1639,7 +2365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="576396712"/>
+        <c:axId val="564858880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1689,7 +2415,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="576392120"/>
+        <c:crossAx val="564851664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1733,13 +2459,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -1801,6 +2520,37 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>iIR</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1848,19 +2598,42 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$10</c:f>
+              <c:f>Sheet1!$C$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> PSNR avg</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="00B050"/>
-            </a:solidFill>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1873,50 +2646,847 @@
             </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$K$11:$K$13</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Normal</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>High</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$69:$B$74</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$11:$L$13</c:f>
+              <c:f>Sheet1!$C$69:$C$74</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>265.2</c:v>
+                  <c:v>220</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>302.60000000000002</c:v>
+                  <c:v>155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>437.6</c:v>
+                  <c:v>627</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>666</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>728</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>206</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-88E0-4920-A449-249E2F483D30}"/>
+              <c16:uniqueId val="{00000000-BECA-4E57-817D-3BF61BC8AEA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$69:$B$74</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$69:$D$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>414</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>504</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>397</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>735</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BECA-4E57-817D-3BF61BC8AEA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent3">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$69:$B$74</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$69:$E$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>422</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>674</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>384</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>390</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-BECA-4E57-817D-3BF61BC8AEA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent4">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent4">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$69:$B$74</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$69:$F$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>352</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>455</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>496</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-BECA-4E57-817D-3BF61BC8AEA1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent5">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent5">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$69:$B$74</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="6"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>PSNR</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>MSE</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$69:$G$74</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>715</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>598</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>773</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-BECA-4E57-817D-3BF61BC8AEA1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
@@ -1924,11 +3494,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="575467168"/>
-        <c:axId val="575472744"/>
+        <c:axId val="564851664"/>
+        <c:axId val="564858880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="575467168"/>
+        <c:axId val="564851664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1970,7 +3540,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="575472744"/>
+        <c:crossAx val="564858880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1978,7 +3548,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="575472744"/>
+        <c:axId val="564858880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2028,7 +3598,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="575467168"/>
+        <c:crossAx val="564851664"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2040,15 +3610,38 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2157,18 +3750,18 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$10</c:f>
+              <c:f>Sheet1!$L$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>MSE avg</c:v>
+                  <c:v> PSNR avg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FF0000"/>
+              <a:srgbClr val="00B050"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -2183,43 +3776,92 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$K$11:$K$13</c:f>
-              <c:strCache>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>Low</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Normal</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>High</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$J$11:$K$19</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Wavelet</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>FIR</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>IIR</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$11:$M$13</c:f>
+              <c:f>Sheet1!$L$11:$L$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>567.20000000000005</c:v>
+                  <c:v>265.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>529</c:v>
+                  <c:v>302.60000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>383.4</c:v>
+                  <c:v>437.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>265.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>302.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>437.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>265.2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>302.60000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>437.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3939-4D4C-A1DE-F2E9309355C6}"/>
+              <c16:uniqueId val="{00000000-8D18-4931-8A5B-6B9442551BBC}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2233,11 +3875,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="513214656"/>
-        <c:axId val="513214328"/>
+        <c:axId val="594651360"/>
+        <c:axId val="594650376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="513214656"/>
+        <c:axId val="594651360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2279,7 +3921,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="513214328"/>
+        <c:crossAx val="594650376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2287,7 +3929,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="513214328"/>
+        <c:axId val="594650376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2337,7 +3979,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="513214656"/>
+        <c:crossAx val="594651360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2351,13 +3993,357 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>MSE avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$J$11:$K$19</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>High</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Low</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Normal</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>High</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Wavelet</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>FIR</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>IIR</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$11:$M$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>567.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>383.4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>567.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>383.4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>567.20000000000005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>529</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>383.4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7078-41F6-B0EC-B006ABD7B3F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="594651360"/>
+        <c:axId val="594650376"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="594651360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594650376"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="594650376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="594651360"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -2445,10 +4431,13 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -2482,9 +4471,12 @@
 </file>
 
 <file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -2558,6 +4550,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
@@ -4047,6 +6079,502 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4582,27 +7110,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>828261</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>53008</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>51486</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>72080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>720587</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>62947</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>523100</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>53030</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="9" name="Chart 8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD7B837C-82AD-4C32-976F-52CE656EB45D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D300689-C7D7-4248-ABCD-3AA91C7A7DD6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4618,27 +7148,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>819978</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>61783</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>30892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>712304</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>162339</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>533397</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>11841</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="7" name="Chart 6">
+        <xdr:cNvPr id="10" name="Chart 9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3DCFA494-A0E3-4C4C-86D4-9685A2CCBB73}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9EBE650D-E909-4DB7-838F-12C497AFC334}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -4655,22 +7187,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>894522</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>44726</xdr:rowOff>
+      <xdr:colOff>319217</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>80319</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>786848</xdr:colOff>
-      <xdr:row>63</xdr:row>
-      <xdr:rowOff>54665</xdr:rowOff>
+      <xdr:colOff>205946</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>43249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF6F77B7-178D-45DC-B998-CF7FDC938BAD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1A52B02-2573-40CD-9390-4A0E0E5DEEEE}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4683,6 +7215,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>306551</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>35034</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>193280</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>181894</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CC93F4E3-A8C9-4AEF-8101-24CDB20E6888}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4988,10 +7558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA975F6-26E6-400B-8BCB-2A6EE02F0EC9}">
-  <dimension ref="A3:X21"/>
+  <dimension ref="A3:X74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="60" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5009,6 +7579,26 @@
       <c r="P3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A8" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="C10" s="1">
         <v>1</v>
@@ -5033,7 +7623,7 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -5053,6 +7643,9 @@
       </c>
       <c r="G11" s="1">
         <v>207</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>2</v>
@@ -5067,7 +7660,7 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
+      <c r="A12" s="4"/>
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
@@ -5086,6 +7679,7 @@
       <c r="G12" s="1">
         <v>80</v>
       </c>
+      <c r="J12" s="4"/>
       <c r="K12" s="1" t="s">
         <v>3</v>
       </c>
@@ -5099,7 +7693,7 @@
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>4</v>
       </c>
@@ -5118,6 +7712,7 @@
       <c r="G13" s="1">
         <v>715</v>
       </c>
+      <c r="J13" s="4"/>
       <c r="K13" s="1" t="s">
         <v>4</v>
       </c>
@@ -5126,13 +7721,13 @@
         <v>437.6</v>
       </c>
       <c r="M13" s="1">
-        <f t="shared" ref="M12:M13" si="0">SUM(C16:G16)/5</f>
+        <f t="shared" ref="M13" si="0">SUM(C16:G16)/5</f>
         <v>383.4</v>
       </c>
       <c r="Q13" s="3"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -5153,9 +7748,23 @@
       <c r="G14" s="1">
         <v>598</v>
       </c>
+      <c r="J14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="1">
+        <f>SUM(C41:G41)/5</f>
+        <v>265.2</v>
+      </c>
+      <c r="M14" s="1">
+        <f>SUM(C44:G44)/5</f>
+        <v>567.20000000000005</v>
+      </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
@@ -5174,9 +7783,21 @@
       <c r="G15" s="1">
         <v>773</v>
       </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L15" s="2">
+        <f>SUM(C42:G42)/5</f>
+        <v>302.60000000000002</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" ref="M15:M16" si="1">SUM(C45:G45)/5</f>
+        <v>529</v>
+      </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
+      <c r="A16" s="4"/>
       <c r="B16" s="1" t="s">
         <v>4</v>
       </c>
@@ -5195,23 +7816,423 @@
       <c r="G16" s="1">
         <v>90</v>
       </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L16" s="2">
+        <f>SUM(C43:G43)/5</f>
+        <v>437.6</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="1"/>
+        <v>383.4</v>
+      </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
+      <c r="A17" s="4"/>
+      <c r="J17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L17" s="1">
+        <f>SUM(C69:G69)/5</f>
+        <v>265.2</v>
+      </c>
+      <c r="M17" s="1">
+        <f>SUM(C72:G72)/5</f>
+        <v>567.20000000000005</v>
+      </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
+      <c r="A18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L18" s="2">
+        <f t="shared" ref="L18:L19" si="2">SUM(C70:G70)/5</f>
+        <v>302.60000000000002</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" ref="M18:M19" si="3">SUM(C73:G73)/5</f>
+        <v>529</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="J19" s="4"/>
+      <c r="K19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L19" s="2">
+        <f t="shared" si="2"/>
+        <v>437.6</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="3"/>
+        <v>383.4</v>
+      </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="Q21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
     </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2</v>
+      </c>
+      <c r="E40" s="2">
+        <v>3</v>
+      </c>
+      <c r="F40" s="2">
+        <v>4</v>
+      </c>
+      <c r="G40" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="2">
+        <v>220</v>
+      </c>
+      <c r="D41" s="2">
+        <v>414</v>
+      </c>
+      <c r="E41" s="2">
+        <v>175</v>
+      </c>
+      <c r="F41" s="2">
+        <v>310</v>
+      </c>
+      <c r="G41" s="2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="4"/>
+      <c r="B42" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="2">
+        <v>155</v>
+      </c>
+      <c r="D42" s="2">
+        <v>504</v>
+      </c>
+      <c r="E42" s="2">
+        <v>422</v>
+      </c>
+      <c r="F42" s="2">
+        <v>352</v>
+      </c>
+      <c r="G42" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="4"/>
+      <c r="B43" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C43" s="2">
+        <v>627</v>
+      </c>
+      <c r="D43" s="3">
+        <v>84</v>
+      </c>
+      <c r="E43" s="2">
+        <v>422</v>
+      </c>
+      <c r="F43" s="2">
+        <v>340</v>
+      </c>
+      <c r="G43" s="2">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C44" s="2">
+        <v>666</v>
+      </c>
+      <c r="D44" s="2">
+        <v>397</v>
+      </c>
+      <c r="E44" s="2">
+        <v>674</v>
+      </c>
+      <c r="F44" s="2">
+        <v>501</v>
+      </c>
+      <c r="G44" s="2">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
+      <c r="B45" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C45" s="2">
+        <v>728</v>
+      </c>
+      <c r="D45" s="2">
+        <v>305</v>
+      </c>
+      <c r="E45" s="2">
+        <v>384</v>
+      </c>
+      <c r="F45" s="2">
+        <v>455</v>
+      </c>
+      <c r="G45" s="2">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C46" s="2">
+        <v>206</v>
+      </c>
+      <c r="D46" s="3">
+        <v>735</v>
+      </c>
+      <c r="E46" s="2">
+        <v>390</v>
+      </c>
+      <c r="F46" s="2">
+        <v>496</v>
+      </c>
+      <c r="G46" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" s="2"/>
+      <c r="B68" s="2"/>
+      <c r="C68" s="2">
+        <v>1</v>
+      </c>
+      <c r="D68" s="2">
+        <v>2</v>
+      </c>
+      <c r="E68" s="2">
+        <v>3</v>
+      </c>
+      <c r="F68" s="2">
+        <v>4</v>
+      </c>
+      <c r="G68" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C69" s="2">
+        <v>220</v>
+      </c>
+      <c r="D69" s="2">
+        <v>414</v>
+      </c>
+      <c r="E69" s="2">
+        <v>175</v>
+      </c>
+      <c r="F69" s="2">
+        <v>310</v>
+      </c>
+      <c r="G69" s="2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A70" s="4"/>
+      <c r="B70" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" s="2">
+        <v>155</v>
+      </c>
+      <c r="D70" s="2">
+        <v>504</v>
+      </c>
+      <c r="E70" s="2">
+        <v>422</v>
+      </c>
+      <c r="F70" s="2">
+        <v>352</v>
+      </c>
+      <c r="G70" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A71" s="4"/>
+      <c r="B71" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C71" s="2">
+        <v>627</v>
+      </c>
+      <c r="D71" s="3">
+        <v>84</v>
+      </c>
+      <c r="E71" s="2">
+        <v>422</v>
+      </c>
+      <c r="F71" s="2">
+        <v>340</v>
+      </c>
+      <c r="G71" s="2">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C72" s="2">
+        <v>666</v>
+      </c>
+      <c r="D72" s="2">
+        <v>397</v>
+      </c>
+      <c r="E72" s="2">
+        <v>674</v>
+      </c>
+      <c r="F72" s="2">
+        <v>501</v>
+      </c>
+      <c r="G72" s="2">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A73" s="4"/>
+      <c r="B73" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C73" s="2">
+        <v>728</v>
+      </c>
+      <c r="D73" s="2">
+        <v>305</v>
+      </c>
+      <c r="E73" s="2">
+        <v>384</v>
+      </c>
+      <c r="F73" s="2">
+        <v>455</v>
+      </c>
+      <c r="G73" s="2">
+        <v>773</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A74" s="4"/>
+      <c r="B74" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C74" s="2">
+        <v>206</v>
+      </c>
+      <c r="D74" s="3">
+        <v>735</v>
+      </c>
+      <c r="E74" s="2">
+        <v>390</v>
+      </c>
+      <c r="F74" s="2">
+        <v>496</v>
+      </c>
+      <c r="G74" s="2">
+        <v>90</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="13">
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="A41:A43"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A66:G67"/>
+    <mergeCell ref="A69:A71"/>
+    <mergeCell ref="A72:A74"/>
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A8:G9"/>
+    <mergeCell ref="A38:G39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>